<commit_message>
Update file submission doc
</commit_message>
<xml_diff>
--- a/files/DatasetColumnHeaderSubmission.xlsx
+++ b/files/DatasetColumnHeaderSubmission.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <r>
       <t xml:space="preserve">Column Header
@@ -33,7 +33,7 @@
       <rPr>
         <i/>
       </rPr>
-      <t>Ex. True/False</t>
+      <t>Ex. Yes, No</t>
     </r>
   </si>
   <si>
@@ -46,6 +46,18 @@
         <i/>
       </rPr>
       <t>Ex: 01/01/2001</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Data Type
+</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+      </rPr>
+      <t>Ex. String, Int64, Date(time), Double</t>
     </r>
   </si>
 </sst>
@@ -103,7 +115,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/worksheetdrawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
 </file>
 
@@ -120,6 +132,7 @@
     <col customWidth="1" min="1" max="1" width="16.43"/>
     <col customWidth="1" min="2" max="2" width="21.43"/>
     <col customWidth="1" min="3" max="3" width="52.29"/>
+    <col customWidth="1" min="4" max="4" width="31.57"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -132,8 +145,16 @@
       <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations>
+    <dataValidation type="list" allowBlank="1" sqref="B2:B44">
+      <formula1>"Yes,No"</formula1>
+    </dataValidation>
+  </dataValidations>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>